<commit_message>
put back to $3, update tkt price
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1056,7 +1056,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="D2" s="2">
         <f t="shared" ref="D2:D21" si="0">$D$24/$A$21</f>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E2" s="1">
         <v>0.9</v>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="D3" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E3" s="1">
         <f>VLOOKUP(B3,List!$A$2:$E$27,3,FALSE)</f>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E4" s="1">
         <v>0.9</v>
@@ -1175,15 +1175,14 @@
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E5" s="1">
         <f>VLOOKUP(B5,List!$A$2:$E$27,3,FALSE)</f>
         <v>0.9</v>
       </c>
       <c r="N5" s="1">
-        <f>N2+N3</f>
-        <v>2.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1198,7 +1197,7 @@
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E6" s="1">
         <v>0.9</v>
@@ -1216,7 +1215,7 @@
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E7" s="1">
         <f>VLOOKUP(B7,List!$A$2:$E$27,3,FALSE)</f>
@@ -1235,7 +1234,7 @@
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E8" s="1">
         <v>0.9</v>
@@ -1253,7 +1252,7 @@
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E9" s="1">
         <f>VLOOKUP(B9,List!$A$2:$E$27,3,FALSE)</f>
@@ -1272,7 +1271,7 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E10" s="1">
         <v>0.9</v>
@@ -1290,7 +1289,7 @@
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E11" s="1">
         <f>VLOOKUP(B11,List!$A$2:$E$27,3,FALSE)</f>
@@ -1309,7 +1308,7 @@
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E12" s="1">
         <v>0.9</v>
@@ -1327,7 +1326,7 @@
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E13" s="1">
         <f>VLOOKUP(B13,List!$A$2:$E$27,3,FALSE)</f>
@@ -1346,7 +1345,7 @@
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E14" s="1">
         <v>0.9</v>
@@ -1364,7 +1363,7 @@
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E15" s="1">
         <f>VLOOKUP(B15,List!$A$2:$E$27,3,FALSE)</f>
@@ -1383,7 +1382,7 @@
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E16" s="1">
         <v>0.9</v>
@@ -1401,7 +1400,7 @@
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E17" s="1">
         <f>VLOOKUP(B17,List!$A$2:$E$27,3,FALSE)</f>
@@ -1420,7 +1419,7 @@
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E18" s="1">
         <v>0.9</v>
@@ -1438,7 +1437,7 @@
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E19" s="1">
         <v>0.9</v>
@@ -1456,7 +1455,7 @@
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E20" s="1">
         <v>5</v>
@@ -1474,7 +1473,7 @@
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
       <c r="E21" s="1">
         <v>5</v>
@@ -1494,16 +1493,16 @@
         <v>41</v>
       </c>
       <c r="E22" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" s="2">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E24" s="1">
         <f>SUM(E2:E22)</f>
-        <v>29.200000000000003</v>
+        <v>31.200000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>